<commit_message>
Partial edit for decay chain.
</commit_message>
<xml_diff>
--- a/11-Parameters/decayCHAINpion.xlsx
+++ b/11-Parameters/decayCHAINpion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/2020296750528/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{5A4D95E3-A054-B54E-8E3D-CF81A7248FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D4D3930-FF7C-5346-B511-B298F3C49C89}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{5A4D95E3-A054-B54E-8E3D-CF81A7248FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9512720E-F144-1F41-A1E6-4B332DF2380E}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="760" windowWidth="27540" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29220" yWindow="500" windowWidth="27540" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="decayCHAINpion" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="30">
   <si>
     <t>Parameter</t>
   </si>
@@ -126,12 +126,6 @@
   </si>
   <si>
     <t>muon</t>
-  </si>
-  <si>
-    <t>Kinetic energy 1</t>
-  </si>
-  <si>
-    <t>Species 1</t>
   </si>
 </sst>
 </file>
@@ -594,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,7 +690,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F4" s="9">
         <v>5000</v>
@@ -742,7 +736,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Partial update for decay chain
</commit_message>
<xml_diff>
--- a/11-Parameters/decayCHAINpion.xlsx
+++ b/11-Parameters/decayCHAINpion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/2020296750528/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{5A4D95E3-A054-B54E-8E3D-CF81A7248FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9512720E-F144-1F41-A1E6-4B332DF2380E}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{5A4D95E3-A054-B54E-8E3D-CF81A7248FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC5A2012-663E-F744-AA64-8F84856499D5}"/>
   <bookViews>
-    <workbookView xWindow="29220" yWindow="500" windowWidth="27540" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="decayCHAINpion" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="33">
   <si>
     <t>Parameter</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>muon</t>
+  </si>
+  <si>
+    <t>neutrino</t>
+  </si>
+  <si>
+    <t>Kinetic energy 1</t>
+  </si>
+  <si>
+    <t>Species 1</t>
   </si>
 </sst>
 </file>
@@ -586,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:H112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -690,7 +699,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F4" s="9">
         <v>5000</v>
@@ -736,7 +745,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>29</v>
@@ -745,76 +754,74 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+      <c r="A7" s="8">
         <v>0</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>0</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F8" s="6">
         <v>0.5</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
-        <v>1</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="G8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F9" s="10">
         <v>4</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="1">
-        <v>6000</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -830,10 +837,10 @@
         <v>23</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="1">
-        <v>600</v>
+        <v>6000</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>9</v>
@@ -841,52 +848,52 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="1">
+        <v>600</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F12" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="11">
-        <v>1</v>
-      </c>
+      <c r="G12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -909,8 +916,7 @@
         <v>10</v>
       </c>
       <c r="H13" s="11">
-        <f>H12+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -934,8 +940,8 @@
         <v>10</v>
       </c>
       <c r="H14" s="11">
-        <f t="shared" ref="H14:H21" si="0">H13+1</f>
-        <v>3</v>
+        <f>H13+1</f>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -959,160 +965,160 @@
         <v>10</v>
       </c>
       <c r="H15" s="11">
+        <f t="shared" ref="H15:H22" si="0">H14+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="11">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="11">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="11">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>2</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="11">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>2</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="11">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="11">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>2</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2</v>
@@ -1134,8 +1140,8 @@
         <v>10</v>
       </c>
       <c r="H22" s="11">
-        <f t="shared" ref="H22:H85" si="1">H21+1</f>
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1159,8 +1165,8 @@
         <v>10</v>
       </c>
       <c r="H23" s="11">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" ref="H23:H86" si="1">H22+1</f>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1185,7 +1191,7 @@
       </c>
       <c r="H24" s="11">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1210,7 +1216,7 @@
       </c>
       <c r="H25" s="11">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1235,7 +1241,7 @@
       </c>
       <c r="H26" s="11">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1260,7 +1266,7 @@
       </c>
       <c r="H27" s="11">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1285,7 +1291,7 @@
       </c>
       <c r="H28" s="11">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1310,7 +1316,7 @@
       </c>
       <c r="H29" s="11">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1335,7 +1341,7 @@
       </c>
       <c r="H30" s="11">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1360,7 +1366,7 @@
       </c>
       <c r="H31" s="11">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1385,7 +1391,7 @@
       </c>
       <c r="H32" s="11">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1410,7 +1416,7 @@
       </c>
       <c r="H33" s="11">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1435,7 +1441,7 @@
       </c>
       <c r="H34" s="11">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1460,7 +1466,7 @@
       </c>
       <c r="H35" s="11">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1485,7 +1491,7 @@
       </c>
       <c r="H36" s="11">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1510,7 +1516,7 @@
       </c>
       <c r="H37" s="11">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1535,7 +1541,7 @@
       </c>
       <c r="H38" s="11">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1560,7 +1566,7 @@
       </c>
       <c r="H39" s="11">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1585,7 +1591,7 @@
       </c>
       <c r="H40" s="11">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1610,7 +1616,7 @@
       </c>
       <c r="H41" s="11">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1635,7 +1641,7 @@
       </c>
       <c r="H42" s="11">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1660,7 +1666,7 @@
       </c>
       <c r="H43" s="11">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1685,7 +1691,7 @@
       </c>
       <c r="H44" s="11">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1710,7 +1716,7 @@
       </c>
       <c r="H45" s="11">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1735,7 +1741,7 @@
       </c>
       <c r="H46" s="11">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -1760,7 +1766,7 @@
       </c>
       <c r="H47" s="11">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -1785,7 +1791,7 @@
       </c>
       <c r="H48" s="11">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1810,7 +1816,7 @@
       </c>
       <c r="H49" s="11">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -1835,7 +1841,7 @@
       </c>
       <c r="H50" s="11">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -1860,7 +1866,7 @@
       </c>
       <c r="H51" s="11">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -1885,7 +1891,7 @@
       </c>
       <c r="H52" s="11">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -1910,7 +1916,7 @@
       </c>
       <c r="H53" s="11">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -1935,7 +1941,7 @@
       </c>
       <c r="H54" s="11">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -1960,7 +1966,7 @@
       </c>
       <c r="H55" s="11">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -1985,7 +1991,7 @@
       </c>
       <c r="H56" s="11">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2010,7 +2016,7 @@
       </c>
       <c r="H57" s="11">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2035,7 +2041,7 @@
       </c>
       <c r="H58" s="11">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2060,7 +2066,7 @@
       </c>
       <c r="H59" s="11">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2085,7 +2091,7 @@
       </c>
       <c r="H60" s="11">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -2110,7 +2116,7 @@
       </c>
       <c r="H61" s="11">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2135,7 +2141,7 @@
       </c>
       <c r="H62" s="11">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2160,7 +2166,7 @@
       </c>
       <c r="H63" s="11">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2185,7 +2191,7 @@
       </c>
       <c r="H64" s="11">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2210,7 +2216,7 @@
       </c>
       <c r="H65" s="11">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2235,7 +2241,7 @@
       </c>
       <c r="H66" s="11">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2260,7 +2266,7 @@
       </c>
       <c r="H67" s="11">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -2285,7 +2291,7 @@
       </c>
       <c r="H68" s="11">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -2310,7 +2316,7 @@
       </c>
       <c r="H69" s="11">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -2335,7 +2341,7 @@
       </c>
       <c r="H70" s="11">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -2360,7 +2366,7 @@
       </c>
       <c r="H71" s="11">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2385,7 +2391,7 @@
       </c>
       <c r="H72" s="11">
         <f t="shared" si="1"/>
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2410,7 +2416,7 @@
       </c>
       <c r="H73" s="11">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -2435,7 +2441,7 @@
       </c>
       <c r="H74" s="11">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -2460,7 +2466,7 @@
       </c>
       <c r="H75" s="11">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -2485,7 +2491,7 @@
       </c>
       <c r="H76" s="11">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -2510,7 +2516,7 @@
       </c>
       <c r="H77" s="11">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2535,7 +2541,7 @@
       </c>
       <c r="H78" s="11">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2560,7 +2566,7 @@
       </c>
       <c r="H79" s="11">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2585,7 +2591,7 @@
       </c>
       <c r="H80" s="11">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2610,7 +2616,7 @@
       </c>
       <c r="H81" s="11">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2635,7 +2641,7 @@
       </c>
       <c r="H82" s="11">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2660,7 +2666,7 @@
       </c>
       <c r="H83" s="11">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -2685,7 +2691,7 @@
       </c>
       <c r="H84" s="11">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -2710,7 +2716,7 @@
       </c>
       <c r="H85" s="11">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -2734,8 +2740,8 @@
         <v>10</v>
       </c>
       <c r="H86" s="11">
-        <f t="shared" ref="H86:H111" si="2">H85+1</f>
-        <v>75</v>
+        <f t="shared" si="1"/>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -2759,606 +2765,631 @@
         <v>10</v>
       </c>
       <c r="H87" s="11">
+        <f t="shared" ref="H87:H112" si="2">H86+1</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>2</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H88" s="11">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="1">
-        <v>2</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F88">
-        <v>1</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H88" s="11">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>2</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H89" s="11">
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="1">
-        <v>2</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F89">
-        <v>1</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H89" s="11">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>2</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H90" s="11">
         <f t="shared" si="2"/>
         <v>78</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="1">
-        <v>2</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F90">
-        <v>1</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H90" s="11">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>2</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H91" s="11">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="1">
-        <v>2</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F91">
-        <v>1</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H91" s="11">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>2</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H92" s="11">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="1">
-        <v>2</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F92">
-        <v>1</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H92" s="11">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>2</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H93" s="11">
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="1">
-        <v>2</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F93">
-        <v>1</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H93" s="11">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>2</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H94" s="11">
         <f t="shared" si="2"/>
         <v>82</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="1">
-        <v>2</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F94">
-        <v>1</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H94" s="11">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>2</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H95" s="11">
         <f t="shared" si="2"/>
         <v>83</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="1">
-        <v>2</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F95">
-        <v>1</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H95" s="11">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>2</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H96" s="11">
         <f t="shared" si="2"/>
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="1">
-        <v>2</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D96" s="1"/>
-      <c r="E96" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F96">
-        <v>1</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H96" s="11">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>2</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97">
+        <v>1</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H97" s="11">
         <f t="shared" si="2"/>
         <v>85</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="1">
-        <v>2</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F97">
-        <v>1</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H97" s="11">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>2</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H98" s="11">
         <f t="shared" si="2"/>
         <v>86</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="1">
-        <v>2</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F98">
-        <v>1</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H98" s="11">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>2</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H99" s="11">
         <f t="shared" si="2"/>
         <v>87</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="1">
-        <v>2</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F99">
-        <v>1</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H99" s="11">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>2</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100">
+        <v>1</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H100" s="11">
         <f t="shared" si="2"/>
         <v>88</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="1">
-        <v>2</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F100">
-        <v>1</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H100" s="11">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>2</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101">
+        <v>1</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H101" s="11">
         <f t="shared" si="2"/>
         <v>89</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="1">
-        <v>2</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F101">
-        <v>1</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H101" s="11">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>2</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F102">
+        <v>1</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H102" s="11">
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="1">
-        <v>2</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F102">
-        <v>1</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H102" s="11">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>2</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F103">
+        <v>1</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H103" s="11">
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="1">
-        <v>2</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F103">
-        <v>1</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H103" s="11">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>2</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F104">
+        <v>1</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H104" s="11">
         <f t="shared" si="2"/>
         <v>92</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="1">
-        <v>2</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F104">
-        <v>1</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H104" s="11">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>2</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F105">
+        <v>1</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H105" s="11">
         <f t="shared" si="2"/>
         <v>93</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="1">
-        <v>2</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F105">
-        <v>1</v>
-      </c>
-      <c r="G105" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H105" s="11">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>2</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F106">
+        <v>1</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H106" s="11">
         <f t="shared" si="2"/>
         <v>94</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="1">
-        <v>2</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F106">
-        <v>1</v>
-      </c>
-      <c r="G106" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H106" s="11">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>2</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F107">
+        <v>1</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H107" s="11">
         <f t="shared" si="2"/>
         <v>95</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="1">
-        <v>2</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D107" s="1"/>
-      <c r="E107" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F107">
-        <v>1</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H107" s="11">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>2</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F108">
+        <v>1</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H108" s="11">
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="1">
-        <v>2</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F108">
-        <v>1</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H108" s="11">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>2</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F109">
+        <v>1</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H109" s="11">
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="1">
-        <v>2</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D109" s="1"/>
-      <c r="E109" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F109">
-        <v>1</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H109" s="11">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>2</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110">
+        <v>1</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H110" s="11">
         <f t="shared" si="2"/>
         <v>98</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="1">
-        <v>2</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F110">
-        <v>1</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H110" s="11">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>2</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111">
+        <v>1</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H111" s="11">
         <f t="shared" si="2"/>
         <v>99</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="2">
-        <v>2</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D111" s="2"/>
-      <c r="E111" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F111" s="12">
-        <v>1</v>
-      </c>
-      <c r="G111" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H111" s="13">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="2">
+        <v>2</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F112" s="12">
+        <v>1</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H112" s="13">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Pion -> muon decay chain
</commit_message>
<xml_diff>
--- a/11-Parameters/decayCHAINpion.xlsx
+++ b/11-Parameters/decayCHAINpion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://api.box.com/wopi/files/2020296750528/WOPIServiceId_TP_BOX_2/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{5A4D95E3-A054-B54E-8E3D-CF81A7248FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC5A2012-663E-F744-AA64-8F84856499D5}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{5A4D95E3-A054-B54E-8E3D-CF81A7248FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB066A1F-EFA8-7747-A7F5-C079B25B9B22}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="15140" windowHeight="18980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="decayCHAINpion" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="34">
   <si>
     <t>Parameter</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Species 1</t>
+  </si>
+  <si>
+    <t>electron</t>
   </si>
 </sst>
 </file>
@@ -595,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,12 +726,14 @@
         <v>18</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="F5" s="9">
+        <v>2000</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -745,10 +750,10 @@
         <v>18</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -770,179 +775,174 @@
         <v>32</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+      <c r="A8" s="8">
         <v>0</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>0</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>0</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F10" s="6">
         <v>0.5</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
-        <v>1</v>
-      </c>
-      <c r="B9" s="10" t="s">
+      <c r="G10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>1</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F11" s="10">
         <v>4</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10" t="s">
+      <c r="G11" s="10"/>
+      <c r="H11" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F12" s="1">
         <v>6000</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="1">
-        <v>600</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="F13" s="1">
+        <v>600</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="11">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="11">
-        <f>H13+1</f>
-        <v>2</v>
-      </c>
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -965,8 +965,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="11">
-        <f t="shared" ref="H15:H22" si="0">H14+1</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -990,185 +989,185 @@
         <v>10</v>
       </c>
       <c r="H16" s="11">
+        <f>H15+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" ref="H17:H24" si="0">H16+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>2</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="11">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="11">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>2</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="11">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>2</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="11">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>2</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="11">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="11">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>2</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>2</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="11">
-        <f t="shared" ref="H23:H86" si="1">H22+1</f>
-        <v>11</v>
-      </c>
-    </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2</v>
@@ -1190,8 +1189,8 @@
         <v>10</v>
       </c>
       <c r="H24" s="11">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1215,8 +1214,8 @@
         <v>10</v>
       </c>
       <c r="H25" s="11">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f t="shared" ref="H25:H88" si="1">H24+1</f>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1241,7 +1240,7 @@
       </c>
       <c r="H26" s="11">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1266,7 +1265,7 @@
       </c>
       <c r="H27" s="11">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1291,7 +1290,7 @@
       </c>
       <c r="H28" s="11">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1316,7 +1315,7 @@
       </c>
       <c r="H29" s="11">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1341,7 +1340,7 @@
       </c>
       <c r="H30" s="11">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1366,7 +1365,7 @@
       </c>
       <c r="H31" s="11">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1391,7 +1390,7 @@
       </c>
       <c r="H32" s="11">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1416,7 +1415,7 @@
       </c>
       <c r="H33" s="11">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1441,7 +1440,7 @@
       </c>
       <c r="H34" s="11">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1466,7 +1465,7 @@
       </c>
       <c r="H35" s="11">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1491,7 +1490,7 @@
       </c>
       <c r="H36" s="11">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1516,7 +1515,7 @@
       </c>
       <c r="H37" s="11">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1541,7 +1540,7 @@
       </c>
       <c r="H38" s="11">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1566,7 +1565,7 @@
       </c>
       <c r="H39" s="11">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1591,7 +1590,7 @@
       </c>
       <c r="H40" s="11">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1616,7 +1615,7 @@
       </c>
       <c r="H41" s="11">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1641,7 +1640,7 @@
       </c>
       <c r="H42" s="11">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1666,7 +1665,7 @@
       </c>
       <c r="H43" s="11">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1691,7 +1690,7 @@
       </c>
       <c r="H44" s="11">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1716,7 +1715,7 @@
       </c>
       <c r="H45" s="11">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1741,7 +1740,7 @@
       </c>
       <c r="H46" s="11">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -1766,7 +1765,7 @@
       </c>
       <c r="H47" s="11">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -1791,7 +1790,7 @@
       </c>
       <c r="H48" s="11">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1816,7 +1815,7 @@
       </c>
       <c r="H49" s="11">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -1841,7 +1840,7 @@
       </c>
       <c r="H50" s="11">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -1866,7 +1865,7 @@
       </c>
       <c r="H51" s="11">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -1891,7 +1890,7 @@
       </c>
       <c r="H52" s="11">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -1916,7 +1915,7 @@
       </c>
       <c r="H53" s="11">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -1941,7 +1940,7 @@
       </c>
       <c r="H54" s="11">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -1966,7 +1965,7 @@
       </c>
       <c r="H55" s="11">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -1991,7 +1990,7 @@
       </c>
       <c r="H56" s="11">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2016,7 +2015,7 @@
       </c>
       <c r="H57" s="11">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2041,7 +2040,7 @@
       </c>
       <c r="H58" s="11">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2066,7 +2065,7 @@
       </c>
       <c r="H59" s="11">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2091,7 +2090,7 @@
       </c>
       <c r="H60" s="11">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -2116,7 +2115,7 @@
       </c>
       <c r="H61" s="11">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2141,7 +2140,7 @@
       </c>
       <c r="H62" s="11">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2166,7 +2165,7 @@
       </c>
       <c r="H63" s="11">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2191,7 +2190,7 @@
       </c>
       <c r="H64" s="11">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2216,7 +2215,7 @@
       </c>
       <c r="H65" s="11">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2241,7 +2240,7 @@
       </c>
       <c r="H66" s="11">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2266,7 +2265,7 @@
       </c>
       <c r="H67" s="11">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -2291,7 +2290,7 @@
       </c>
       <c r="H68" s="11">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -2316,7 +2315,7 @@
       </c>
       <c r="H69" s="11">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -2341,7 +2340,7 @@
       </c>
       <c r="H70" s="11">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -2366,7 +2365,7 @@
       </c>
       <c r="H71" s="11">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2391,7 +2390,7 @@
       </c>
       <c r="H72" s="11">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2416,7 +2415,7 @@
       </c>
       <c r="H73" s="11">
         <f t="shared" si="1"/>
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -2441,7 +2440,7 @@
       </c>
       <c r="H74" s="11">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -2466,7 +2465,7 @@
       </c>
       <c r="H75" s="11">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -2491,7 +2490,7 @@
       </c>
       <c r="H76" s="11">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -2516,7 +2515,7 @@
       </c>
       <c r="H77" s="11">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2541,7 +2540,7 @@
       </c>
       <c r="H78" s="11">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2566,7 +2565,7 @@
       </c>
       <c r="H79" s="11">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2591,7 +2590,7 @@
       </c>
       <c r="H80" s="11">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2616,7 +2615,7 @@
       </c>
       <c r="H81" s="11">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2641,7 +2640,7 @@
       </c>
       <c r="H82" s="11">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2666,7 +2665,7 @@
       </c>
       <c r="H83" s="11">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -2691,7 +2690,7 @@
       </c>
       <c r="H84" s="11">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -2716,7 +2715,7 @@
       </c>
       <c r="H85" s="11">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -2741,7 +2740,7 @@
       </c>
       <c r="H86" s="11">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -2765,8 +2764,8 @@
         <v>10</v>
       </c>
       <c r="H87" s="11">
-        <f t="shared" ref="H87:H112" si="2">H86+1</f>
-        <v>75</v>
+        <f t="shared" si="1"/>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -2790,606 +2789,656 @@
         <v>10</v>
       </c>
       <c r="H88" s="11">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>2</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H89" s="11">
+        <f t="shared" ref="H89:H114" si="2">H88+1</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>2</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H90" s="11">
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="1">
-        <v>2</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F89">
-        <v>1</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H89" s="11">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>2</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H91" s="11">
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="1">
-        <v>2</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F90">
-        <v>1</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H90" s="11">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>2</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H92" s="11">
         <f t="shared" si="2"/>
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="1">
-        <v>2</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F91">
-        <v>1</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H91" s="11">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>2</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H93" s="11">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="1">
-        <v>2</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F92">
-        <v>1</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H92" s="11">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>2</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H94" s="11">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="1">
-        <v>2</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F93">
-        <v>1</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H93" s="11">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>2</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H95" s="11">
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="1">
-        <v>2</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F94">
-        <v>1</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H94" s="11">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>2</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H96" s="11">
         <f t="shared" si="2"/>
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="1">
-        <v>2</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F95">
-        <v>1</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H95" s="11">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>2</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97">
+        <v>1</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H97" s="11">
         <f t="shared" si="2"/>
         <v>83</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="1">
-        <v>2</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D96" s="1"/>
-      <c r="E96" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F96">
-        <v>1</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H96" s="11">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>2</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H98" s="11">
         <f t="shared" si="2"/>
         <v>84</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="1">
-        <v>2</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F97">
-        <v>1</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H97" s="11">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>2</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H99" s="11">
         <f t="shared" si="2"/>
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="1">
-        <v>2</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F98">
-        <v>1</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H98" s="11">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>2</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100">
+        <v>1</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H100" s="11">
         <f t="shared" si="2"/>
         <v>86</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="1">
-        <v>2</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F99">
-        <v>1</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H99" s="11">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>2</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101">
+        <v>1</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H101" s="11">
         <f t="shared" si="2"/>
         <v>87</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="1">
-        <v>2</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F100">
-        <v>1</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H100" s="11">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>2</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F102">
+        <v>1</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H102" s="11">
         <f t="shared" si="2"/>
         <v>88</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="1">
-        <v>2</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F101">
-        <v>1</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H101" s="11">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>2</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F103">
+        <v>1</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H103" s="11">
         <f t="shared" si="2"/>
         <v>89</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="1">
-        <v>2</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F102">
-        <v>1</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H102" s="11">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>2</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F104">
+        <v>1</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H104" s="11">
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="1">
-        <v>2</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F103">
-        <v>1</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H103" s="11">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>2</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F105">
+        <v>1</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H105" s="11">
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="1">
-        <v>2</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F104">
-        <v>1</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H104" s="11">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>2</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F106">
+        <v>1</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H106" s="11">
         <f t="shared" si="2"/>
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="1">
-        <v>2</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F105">
-        <v>1</v>
-      </c>
-      <c r="G105" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H105" s="11">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>2</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F107">
+        <v>1</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H107" s="11">
         <f t="shared" si="2"/>
         <v>93</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="1">
-        <v>2</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F106">
-        <v>1</v>
-      </c>
-      <c r="G106" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H106" s="11">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>2</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F108">
+        <v>1</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H108" s="11">
         <f t="shared" si="2"/>
         <v>94</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="1">
-        <v>2</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D107" s="1"/>
-      <c r="E107" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F107">
-        <v>1</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H107" s="11">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>2</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F109">
+        <v>1</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H109" s="11">
         <f t="shared" si="2"/>
         <v>95</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="1">
-        <v>2</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F108">
-        <v>1</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H108" s="11">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>2</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110">
+        <v>1</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H110" s="11">
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="1">
-        <v>2</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D109" s="1"/>
-      <c r="E109" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F109">
-        <v>1</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H109" s="11">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>2</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111">
+        <v>1</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H111" s="11">
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="1">
-        <v>2</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F110">
-        <v>1</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H110" s="11">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>2</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F112">
+        <v>1</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H112" s="11">
         <f t="shared" si="2"/>
         <v>98</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="1">
-        <v>2</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D111" s="1"/>
-      <c r="E111" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F111">
-        <v>1</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H111" s="11">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>2</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F113">
+        <v>1</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H113" s="11">
         <f t="shared" si="2"/>
         <v>99</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="2">
-        <v>2</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D112" s="2"/>
-      <c r="E112" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F112" s="12">
-        <v>1</v>
-      </c>
-      <c r="G112" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H112" s="13">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
+        <v>2</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F114" s="12">
+        <v>1</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H114" s="13">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>

</xml_diff>